<commit_message>
adding detailed pop raw data
</commit_message>
<xml_diff>
--- a/raw_data/national/national_dta.xlsx
+++ b/raw_data/national/national_dta.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonoshah/quick_stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/temp/AAPIData_quickstats_master/raw_data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="14220" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="edu" sheetId="5" r:id="rId1"/>
     <sheet name="cvap" sheetId="4" r:id="rId2"/>
     <sheet name="lep" sheetId="6" r:id="rId3"/>
-    <sheet name="nativity" sheetId="7" r:id="rId4"/>
+    <sheet name="pop" sheetId="8" r:id="rId4"/>
+    <sheet name="nativity" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="115">
   <si>
     <t>total_pop</t>
   </si>
@@ -366,6 +367,15 @@
   </si>
   <si>
     <t>pct_foreign</t>
+  </si>
+  <si>
+    <t>popgroupid</t>
+  </si>
+  <si>
+    <t>est_national_pop</t>
+  </si>
+  <si>
+    <t>pct_pop</t>
   </si>
 </sst>
 </file>
@@ -8535,9 +8545,1896 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>316515008</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>316515008</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>39908096</v>
+      </c>
+      <c r="E3">
+        <v>26702</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>316515008</v>
+      </c>
+      <c r="H3">
+        <v>0.12608595192432404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>2569170</v>
+      </c>
+      <c r="E4">
+        <v>14914</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>316515008</v>
+      </c>
+      <c r="H4">
+        <v>8.1170555204153061E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>16235305</v>
+      </c>
+      <c r="E5">
+        <v>20725</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>316515008</v>
+      </c>
+      <c r="H5">
+        <v>5.1293950527906418E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>3303512</v>
+      </c>
+      <c r="E6">
+        <v>17090</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>316515008</v>
+      </c>
+      <c r="H6">
+        <v>1.0437142103910446E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>153234</v>
+      </c>
+      <c r="E7">
+        <v>5479</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>316515008</v>
+      </c>
+      <c r="H7">
+        <v>4.8412871547043324E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>263396</v>
+      </c>
+      <c r="E8">
+        <v>8409</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>316515008</v>
+      </c>
+      <c r="H8">
+        <v>8.321753703057766E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>3852099</v>
+      </c>
+      <c r="E9">
+        <v>19831</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>316515008</v>
+      </c>
+      <c r="H9">
+        <v>1.2170352041721344E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>3693977</v>
+      </c>
+      <c r="E10">
+        <v>18855</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>316515008</v>
+      </c>
+      <c r="H10">
+        <v>1.1670780368149281E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>148275</v>
+      </c>
+      <c r="E11">
+        <v>4247</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>316515008</v>
+      </c>
+      <c r="H11">
+        <v>4.6846119221299887E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>2717844</v>
+      </c>
+      <c r="E12">
+        <v>17934</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>316515008</v>
+      </c>
+      <c r="H12">
+        <v>8.5867773741483688E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>267009</v>
+      </c>
+      <c r="E13">
+        <v>6734</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>316515008</v>
+      </c>
+      <c r="H13">
+        <v>8.4359035827219486E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>71451</v>
+      </c>
+      <c r="E14">
+        <v>2920</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>316515008</v>
+      </c>
+      <c r="H14">
+        <v>2.2574285685550421E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>779637</v>
+      </c>
+      <c r="E15">
+        <v>9694</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>316515008</v>
+      </c>
+      <c r="H15">
+        <v>2.463191282004118E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>1460214</v>
+      </c>
+      <c r="E16">
+        <v>13339</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>316515008</v>
+      </c>
+      <c r="H16">
+        <v>4.6134116128087044E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>207999</v>
+      </c>
+      <c r="E17">
+        <v>4997</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>316515008</v>
+      </c>
+      <c r="H17">
+        <v>6.5715366508811712E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>18803</v>
+      </c>
+      <c r="E18">
+        <v>1544</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>316515008</v>
+      </c>
+      <c r="H18">
+        <v>5.940634582657367E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19">
+        <v>26</v>
+      </c>
+      <c r="D19">
+        <v>414880</v>
+      </c>
+      <c r="E19">
+        <v>11430</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>316515008</v>
+      </c>
+      <c r="H19">
+        <v>1.3107751728966832E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20">
+        <v>27</v>
+      </c>
+      <c r="D20">
+        <v>46036</v>
+      </c>
+      <c r="E20">
+        <v>2724</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>316515008</v>
+      </c>
+      <c r="H20">
+        <v>1.4544649457093328E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>188673</v>
+      </c>
+      <c r="E21">
+        <v>4784</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>316515008</v>
+      </c>
+      <c r="H21">
+        <v>5.9609493473544717E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>1710547</v>
+      </c>
+      <c r="E22">
+        <v>18780</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>316515008</v>
+      </c>
+      <c r="H22">
+        <v>5.404315423220396E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>19167716</v>
+      </c>
+      <c r="E23">
+        <v>19485</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>316515008</v>
+      </c>
+      <c r="H23">
+        <v>6.0558632016181946E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>3590279</v>
+      </c>
+      <c r="E24">
+        <v>16777</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>316515008</v>
+      </c>
+      <c r="H24">
+        <v>1.1343155987560749E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>164821</v>
+      </c>
+      <c r="E25">
+        <v>5618</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>316515008</v>
+      </c>
+      <c r="H25">
+        <v>5.2073673577979207E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>316640</v>
+      </c>
+      <c r="E26">
+        <v>8596</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>316515008</v>
+      </c>
+      <c r="H26">
+        <v>1.0003949282690883E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27">
+        <v>35</v>
+      </c>
+      <c r="D27">
+        <v>4597905</v>
+      </c>
+      <c r="E27">
+        <v>24921</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>316515008</v>
+      </c>
+      <c r="H27">
+        <v>1.4526656828820705E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>4428363</v>
+      </c>
+      <c r="E28">
+        <v>23401</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>316515008</v>
+      </c>
+      <c r="H28">
+        <v>1.3991004787385464E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <v>37</v>
+      </c>
+      <c r="D29">
+        <v>181029</v>
+      </c>
+      <c r="E29">
+        <v>4898</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>316515008</v>
+      </c>
+      <c r="H29">
+        <v>5.7194445980712771E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>3707082</v>
+      </c>
+      <c r="E30">
+        <v>24374</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>316515008</v>
+      </c>
+      <c r="H30">
+        <v>1.1712184175848961E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31">
+        <v>39</v>
+      </c>
+      <c r="D31">
+        <v>280410</v>
+      </c>
+      <c r="E31">
+        <v>6971</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>316515008</v>
+      </c>
+      <c r="H31">
+        <v>8.8592956308275461E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32">
+        <v>40</v>
+      </c>
+      <c r="D32">
+        <v>108477</v>
+      </c>
+      <c r="E32">
+        <v>3749</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>316515008</v>
+      </c>
+      <c r="H32">
+        <v>3.4272309858351946E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33">
+        <v>41</v>
+      </c>
+      <c r="D33">
+        <v>1388163</v>
+      </c>
+      <c r="E33">
+        <v>15805</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>316515008</v>
+      </c>
+      <c r="H33">
+        <v>4.385773092508316E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>1792437</v>
+      </c>
+      <c r="E34">
+        <v>14297</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>316515008</v>
+      </c>
+      <c r="H34">
+        <v>5.6630396284162998E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35">
+        <v>43</v>
+      </c>
+      <c r="D35">
+        <v>256416</v>
+      </c>
+      <c r="E35">
+        <v>5432</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>316515008</v>
+      </c>
+      <c r="H35">
+        <v>8.1012269947677851E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36">
+        <v>44</v>
+      </c>
+      <c r="D36">
+        <v>28818</v>
+      </c>
+      <c r="E36">
+        <v>1890</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>316515008</v>
+      </c>
+      <c r="H36">
+        <v>9.1047812020406127E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37">
+        <v>45</v>
+      </c>
+      <c r="D37">
+        <v>455005</v>
+      </c>
+      <c r="E37">
+        <v>11349</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>316515008</v>
+      </c>
+      <c r="H37">
+        <v>1.4375463360920548E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38">
+        <v>46</v>
+      </c>
+      <c r="D38">
+        <v>52267</v>
+      </c>
+      <c r="E38">
+        <v>2925</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>316515008</v>
+      </c>
+      <c r="H38">
+        <v>1.6513277660124004E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39">
+        <v>47</v>
+      </c>
+      <c r="D39">
+        <v>278281</v>
+      </c>
+      <c r="E39">
+        <v>5520</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>316515008</v>
+      </c>
+      <c r="H39">
+        <v>8.7920320220291615E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40">
+        <v>48</v>
+      </c>
+      <c r="D40">
+        <v>1928363</v>
+      </c>
+      <c r="E40">
+        <v>19234</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>316515008</v>
+      </c>
+      <c r="H40">
+        <v>6.0924850404262543E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="D41">
+        <v>546255</v>
+      </c>
+      <c r="E41">
+        <v>4552</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>316515008</v>
+      </c>
+      <c r="H41">
+        <v>1.7258423613384366E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42">
+        <v>51</v>
+      </c>
+      <c r="D42">
+        <v>344487</v>
+      </c>
+      <c r="E42">
+        <v>4839</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>316515008</v>
+      </c>
+      <c r="H42">
+        <v>1.0883748764172196E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43">
+        <v>52</v>
+      </c>
+      <c r="D43">
+        <v>174460</v>
+      </c>
+      <c r="E43">
+        <v>4519</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>316515008</v>
+      </c>
+      <c r="H43">
+        <v>5.5119028547778726E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44">
+        <v>53</v>
+      </c>
+      <c r="D44">
+        <v>109455</v>
+      </c>
+      <c r="E44">
+        <v>3835</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>316515008</v>
+      </c>
+      <c r="H44">
+        <v>3.4581299405544996E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45">
+        <v>54</v>
+      </c>
+      <c r="D45">
+        <v>45453</v>
+      </c>
+      <c r="E45">
+        <v>2981</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>316515008</v>
+      </c>
+      <c r="H45">
+        <v>1.4360457134898752E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46">
+        <v>55</v>
+      </c>
+      <c r="D46">
+        <v>138360</v>
+      </c>
+      <c r="E46">
+        <v>3689</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>316515008</v>
+      </c>
+      <c r="H46">
+        <v>4.3713566265068948E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47">
+        <v>56</v>
+      </c>
+      <c r="D47">
+        <v>73088</v>
+      </c>
+      <c r="E47">
+        <v>2797</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>316515008</v>
+      </c>
+      <c r="H47">
+        <v>2.3091479670256376E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48">
+        <v>57</v>
+      </c>
+      <c r="D48">
+        <v>34239</v>
+      </c>
+      <c r="E48">
+        <v>1993</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>316515008</v>
+      </c>
+      <c r="H48">
+        <v>1.0817496513482183E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49">
+        <v>58</v>
+      </c>
+      <c r="D49">
+        <v>33468</v>
+      </c>
+      <c r="E49">
+        <v>1972</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>316515008</v>
+      </c>
+      <c r="H49">
+        <v>1.0573906183708459E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50">
+        <v>60</v>
+      </c>
+      <c r="D50">
+        <v>1262434</v>
+      </c>
+      <c r="E50">
+        <v>9700</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>316515008</v>
+      </c>
+      <c r="H50">
+        <v>3.9885439909994602E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51">
+        <v>61</v>
+      </c>
+      <c r="D51">
+        <v>783326</v>
+      </c>
+      <c r="E51">
+        <v>7279</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>316515008</v>
+      </c>
+      <c r="H51">
+        <v>2.4748463183641434E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52">
+        <v>62</v>
+      </c>
+      <c r="D52">
+        <v>549858</v>
+      </c>
+      <c r="E52">
+        <v>8077</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>316515008</v>
+      </c>
+      <c r="H52">
+        <v>1.7372256843373179E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53">
+        <v>63</v>
+      </c>
+      <c r="D53">
+        <v>182968</v>
+      </c>
+      <c r="E53">
+        <v>5079</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>316515008</v>
+      </c>
+      <c r="H53">
+        <v>5.7807052507996559E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54">
+        <v>64</v>
+      </c>
+      <c r="D54">
+        <v>62458</v>
+      </c>
+      <c r="E54">
+        <v>3119</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>316515008</v>
+      </c>
+      <c r="H54">
+        <v>1.9733030057977885E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55">
+        <v>65</v>
+      </c>
+      <c r="D55">
+        <v>207128</v>
+      </c>
+      <c r="E55">
+        <v>4178</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>316515008</v>
+      </c>
+      <c r="H55">
+        <v>6.5440183971077204E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56">
+        <v>66</v>
+      </c>
+      <c r="D56">
+        <v>130476</v>
+      </c>
+      <c r="E56">
+        <v>3970</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>316515008</v>
+      </c>
+      <c r="H56">
+        <v>4.1222688741981983E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57">
+        <v>67</v>
+      </c>
+      <c r="D57">
+        <v>43211</v>
+      </c>
+      <c r="E57">
+        <v>2222</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>316515008</v>
+      </c>
+      <c r="H57">
+        <v>1.3652117922902107E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58">
+        <v>68</v>
+      </c>
+      <c r="D58">
+        <v>42110</v>
+      </c>
+      <c r="E58">
+        <v>2220</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>316515008</v>
+      </c>
+      <c r="H58">
+        <v>1.330426603090018E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59">
+        <v>72</v>
+      </c>
+      <c r="D59">
+        <v>21441</v>
+      </c>
+      <c r="E59">
+        <v>2416</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>316515008</v>
+      </c>
+      <c r="H59">
+        <v>6.77408606861718E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60">
+        <v>73</v>
+      </c>
+      <c r="D60">
+        <v>126590</v>
+      </c>
+      <c r="E60">
+        <v>5388</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>316515008</v>
+      </c>
+      <c r="H60">
+        <v>3.9994943654164672E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61">
+        <v>75</v>
+      </c>
+      <c r="D61">
+        <v>15919</v>
+      </c>
+      <c r="E61">
+        <v>1626</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>316515008</v>
+      </c>
+      <c r="H61">
+        <v>5.0294613174628466E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62">
+        <v>76</v>
+      </c>
+      <c r="D62">
+        <v>103526</v>
+      </c>
+      <c r="E62">
+        <v>4285</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>316515008</v>
+      </c>
+      <c r="H62">
+        <v>3.2708086655475199E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63">
+        <v>80</v>
+      </c>
+      <c r="D63">
+        <v>24875</v>
+      </c>
+      <c r="E63">
+        <v>2425</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>316515008</v>
+      </c>
+      <c r="H63">
+        <v>7.8590266639366746E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64">
+        <v>81</v>
+      </c>
+      <c r="D64">
+        <v>138426</v>
+      </c>
+      <c r="E64">
+        <v>5576</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>316515008</v>
+      </c>
+      <c r="H64">
+        <v>4.3734419159591198E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65">
+        <v>83</v>
+      </c>
+      <c r="D65">
+        <v>20546</v>
+      </c>
+      <c r="E65">
+        <v>1898</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>316515008</v>
+      </c>
+      <c r="H65">
+        <v>6.4913190726656467E-5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66">
+        <v>84</v>
+      </c>
+      <c r="D66">
+        <v>111021</v>
+      </c>
+      <c r="E66">
+        <v>4578</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>316515008</v>
+      </c>
+      <c r="H66">
+        <v>3.5076061612926424E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67">
+        <v>85</v>
+      </c>
+      <c r="D67">
+        <v>11627</v>
+      </c>
+      <c r="E67">
+        <v>870</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>316515008</v>
+      </c>
+      <c r="H67">
+        <v>3.6734436434926465E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68">
+        <v>96</v>
+      </c>
+      <c r="D68">
+        <v>23444</v>
+      </c>
+      <c r="E68">
+        <v>1988</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>316515008</v>
+      </c>
+      <c r="H68">
+        <v>7.4069161200895905E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69">
+        <v>176</v>
+      </c>
+      <c r="D69">
+        <v>26856</v>
+      </c>
+      <c r="E69">
+        <v>2368</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>316515008</v>
+      </c>
+      <c r="H69">
+        <v>8.4849059931002557E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70">
+        <v>177</v>
+      </c>
+      <c r="D70">
+        <v>8957</v>
+      </c>
+      <c r="E70">
+        <v>1133</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>316515008</v>
+      </c>
+      <c r="H70">
+        <v>2.8298816687311046E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71">
+        <v>400</v>
+      </c>
+      <c r="D71">
+        <v>54232204</v>
+      </c>
+      <c r="E71">
+        <v>2036</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>316515008</v>
+      </c>
+      <c r="H71">
+        <v>0.1713416576385498</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72">
+        <v>451</v>
+      </c>
+      <c r="D72">
+        <v>197258272</v>
+      </c>
+      <c r="E72">
+        <v>8320</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>316515008</v>
+      </c>
+      <c r="H72">
+        <v>0.62321931123733521</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed the coding problems
</commit_message>
<xml_diff>
--- a/raw_data/national/national_dta.xlsx
+++ b/raw_data/national/national_dta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="14220" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14220" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="edu" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="114">
   <si>
     <t>total_pop</t>
   </si>
@@ -367,9 +367,6 @@
   </si>
   <si>
     <t>pct_foreign</t>
-  </si>
-  <si>
-    <t>popgroupid</t>
   </si>
   <si>
     <t>est_national_pop</t>
@@ -8548,7 +8545,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H72"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8561,7 +8558,7 @@
         <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
         <v>105</v>
@@ -8573,10 +8570,10 @@
         <v>107</v>
       </c>
       <c r="G1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" t="s">
         <v>113</v>
-      </c>
-      <c r="H1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>